<commit_message>
noter fra møde på timeline
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emila\Documents\Github\Afgangsprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEE9390-1B95-44E4-86DE-F385B7719414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716467FB-AF01-4981-9BD5-6E3C98206EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25410" yWindow="1560" windowWidth="28620" windowHeight="13560" xr2:uid="{581C5342-7C54-420F-B1DC-4DB9E8C08EB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{581C5342-7C54-420F-B1DC-4DB9E8C08EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Opgave</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Design LQR controller</t>
   </si>
   <si>
-    <t>Test af system med mobil robot</t>
-  </si>
-  <si>
     <t>Design objektdetektering</t>
   </si>
   <si>
@@ -85,13 +82,16 @@
   </si>
   <si>
     <t>Skriv rapport</t>
+  </si>
+  <si>
+    <t>Benyt sensor data Lidar til at tage handlinger for Robot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,13 +99,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,14 +135,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="God" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,12 +464,12 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="1" max="1" width="64.7109375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
@@ -462,24 +486,24 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>44456</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>44456</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -487,7 +511,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>44470</v>
       </c>
       <c r="C4" t="s">
@@ -495,33 +519,33 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>44470</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>44470</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44470</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>44456</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -529,21 +553,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44484</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44470</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44500</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44484</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -551,9 +575,9 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3">
         <v>44500</v>
       </c>
       <c r="C10" t="s">
@@ -562,10 +586,24 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44500</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
         <v>44531</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>